<commit_message>
adiciona informações sobre as peças (tipo e delay)
</commit_message>
<xml_diff>
--- a/R/prototipo-titulo-tetris.xlsx
+++ b/R/prototipo-titulo-tetris.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiago/Documents/github/divida/experimentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiago/Documents/github/divida/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26043A0-35AF-F846-B8B0-52038EC5040B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AB4323-13AD-844B-9D6D-5E08F262ECB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14180" xr2:uid="{6D50AE37-2286-4040-A4A1-F04AFF384EA6}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14180" activeTab="1" xr2:uid="{6D50AE37-2286-4040-A4A1-F04AFF384EA6}"/>
   </bookViews>
   <sheets>
     <sheet name="tetris" sheetId="1" r:id="rId1"/>
+    <sheet name="tab-tipos" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">tetris!$A$1:$AP$22</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="110">
   <si>
     <t>a</t>
   </si>
@@ -310,6 +311,63 @@
   </si>
   <si>
     <t>col41</t>
+  </si>
+  <si>
+    <t>piece</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>delay</t>
+  </si>
+  <si>
+    <t>J-block</t>
+  </si>
+  <si>
+    <t>I-block</t>
+  </si>
+  <si>
+    <t>O-block</t>
+  </si>
+  <si>
+    <t>L-block</t>
+  </si>
+  <si>
+    <t>Z-block</t>
+  </si>
+  <si>
+    <t>S-block</t>
+  </si>
+  <si>
+    <t>T-block</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -388,7 +446,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -459,11 +517,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -478,6 +545,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,8 +867,8 @@
   </sheetPr>
   <dimension ref="A1:AO52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AN6" sqref="AN6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -963,6 +1033,9 @@
       <c r="AB3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="AG3" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="AH3" s="3" t="s">
         <v>11</v>
       </c>
@@ -970,9 +1043,6 @@
         <v>11</v>
       </c>
       <c r="AJ3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1013,10 +1083,10 @@
       <c r="AC4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AG4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AK4" s="4" t="s">
+      <c r="AJ4" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1048,20 +1118,19 @@
       <c r="Z5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="3" t="s">
+      <c r="AC5" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="AG5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AH5" s="1" t="s">
-        <v>12</v>
+      <c r="AJ5" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="AK5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AL5" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1093,14 +1162,13 @@
       <c r="Z6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AC6" s="6"/>
-      <c r="AD6" s="3" t="s">
+      <c r="AC6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AG6" s="1" t="s">
+      <c r="AF6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AL6" s="7" t="s">
+      <c r="AK6" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1126,9 +1194,11 @@
       <c r="Z7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="3" t="s">
+      <c r="AC7" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="AF7" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="AG7" s="9" t="s">
         <v>14</v>
@@ -1136,16 +1206,13 @@
       <c r="AH7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AI7" s="9" t="s">
-        <v>14</v>
+      <c r="AI7" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="AJ7" s="10" t="s">
         <v>17</v>
       </c>
       <c r="AK7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL7" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1171,26 +1238,25 @@
       <c r="Z8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="3" t="s">
+      <c r="AC8" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="AF8" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="AG8" s="9" t="s">
         <v>15</v>
       </c>
       <c r="AH8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI8" s="9" t="s">
         <v>14</v>
       </c>
+      <c r="AI8" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="AJ8" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AK8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="AL8" s="10" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1231,11 +1297,11 @@
       <c r="AC9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AG9" s="9" t="s">
+      <c r="AF9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AK9" s="11"/>
-      <c r="AL9" s="10" t="s">
+      <c r="AJ9" s="11"/>
+      <c r="AK9" s="10" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1270,11 +1336,11 @@
       <c r="AB10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AG10" s="9" t="s">
+      <c r="AF10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AK10" s="11"/>
-      <c r="AL10" s="10" t="s">
+      <c r="AJ10" s="11"/>
+      <c r="AK10" s="10" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1723,4 +1789,679 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="76" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F73A6D-EB33-8444-8FF2-9E41F99DB41F}">
+  <dimension ref="A1:C60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C59" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C60" s="6">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
gera padrão para ser usado como separator
</commit_message>
<xml_diff>
--- a/R/prototipo-titulo-tetris.xlsx
+++ b/R/prototipo-titulo-tetris.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiago/Documents/github/divida/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100033FE-3F90-1246-9772-8D3265D2DD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4364C446-BD7F-DC44-A702-35A9D7AF8A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14180" activeTab="1" xr2:uid="{6D50AE37-2286-4040-A4A1-F04AFF384EA6}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14180" activeTab="3" xr2:uid="{6D50AE37-2286-4040-A4A1-F04AFF384EA6}"/>
   </bookViews>
   <sheets>
     <sheet name="tetris" sheetId="1" r:id="rId1"/>
     <sheet name="tab-tipos" sheetId="2" r:id="rId2"/>
+    <sheet name="separator" sheetId="3" r:id="rId3"/>
+    <sheet name="separator2" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">tetris!$A$1:$AP$22</definedName>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="136">
   <si>
     <t>a</t>
   </si>
@@ -377,6 +379,75 @@
   </si>
   <si>
     <t>1-1</t>
+  </si>
+  <si>
+    <t>col42</t>
+  </si>
+  <si>
+    <t>col43</t>
+  </si>
+  <si>
+    <t>col44</t>
+  </si>
+  <si>
+    <t>col45</t>
+  </si>
+  <si>
+    <t>col46</t>
+  </si>
+  <si>
+    <t>col47</t>
+  </si>
+  <si>
+    <t>col48</t>
+  </si>
+  <si>
+    <t>col49</t>
+  </si>
+  <si>
+    <t>col50</t>
+  </si>
+  <si>
+    <t>col51</t>
+  </si>
+  <si>
+    <t>col52</t>
+  </si>
+  <si>
+    <t>col53</t>
+  </si>
+  <si>
+    <t>col54</t>
+  </si>
+  <si>
+    <t>col55</t>
+  </si>
+  <si>
+    <t>col56</t>
+  </si>
+  <si>
+    <t>col57</t>
+  </si>
+  <si>
+    <t>col58</t>
+  </si>
+  <si>
+    <t>col59</t>
+  </si>
+  <si>
+    <t>col60</t>
+  </si>
+  <si>
+    <t>col61</t>
+  </si>
+  <si>
+    <t>col62</t>
+  </si>
+  <si>
+    <t>col63</t>
+  </si>
+  <si>
+    <t>col64</t>
   </si>
 </sst>
 </file>
@@ -455,7 +526,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -535,11 +606,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -558,6 +642,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,7 +966,7 @@
   <dimension ref="A1:AO52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AN6" sqref="AN6"/>
+      <selection sqref="A1:AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1805,7 +1893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F73A6D-EB33-8444-8FF2-9E41F99DB41F}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -2474,4 +2562,999 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE831C38-89AC-1B4E-B634-B5C1C2F268E2}">
+  <dimension ref="A1:BJ5"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.83203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:62" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" t="s">
+        <v>69</v>
+      </c>
+      <c r="U1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V1" t="s">
+        <v>71</v>
+      </c>
+      <c r="W1" t="s">
+        <v>72</v>
+      </c>
+      <c r="X1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>123</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>125</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>127</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>128</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>129</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>130</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>131</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>132</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:62" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="4">
+        <v>5</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AT3" s="4">
+        <v>5</v>
+      </c>
+      <c r="BE3" s="1">
+        <v>3</v>
+      </c>
+      <c r="BI3" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:62" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="4">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="2">
+        <v>3</v>
+      </c>
+      <c r="N4" s="1">
+        <v>3</v>
+      </c>
+      <c r="O4" s="4">
+        <v>5</v>
+      </c>
+      <c r="P4" s="4">
+        <v>5</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="U4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG4" s="4">
+        <v>5</v>
+      </c>
+      <c r="AH4" s="5">
+        <v>5</v>
+      </c>
+      <c r="AI4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR4" s="2">
+        <v>3</v>
+      </c>
+      <c r="AS4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AT4" s="4">
+        <v>5</v>
+      </c>
+      <c r="AU4" s="4">
+        <v>5</v>
+      </c>
+      <c r="AW4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AY4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AZ4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="BA4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="BD4" s="1">
+        <v>3</v>
+      </c>
+      <c r="BE4" s="1">
+        <v>3</v>
+      </c>
+      <c r="BI4" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:62" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="1">
+        <v>3</v>
+      </c>
+      <c r="O5" s="1">
+        <v>3</v>
+      </c>
+      <c r="P5" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="T5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="U5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="X5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF5" s="4">
+        <v>5</v>
+      </c>
+      <c r="AG5" s="4">
+        <v>5</v>
+      </c>
+      <c r="AH5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AM5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AO5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AP5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AT5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AU5" s="4">
+        <v>5</v>
+      </c>
+      <c r="AV5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AY5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AZ5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="BA5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="BB5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="BC5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="BD5" s="2">
+        <v>3</v>
+      </c>
+      <c r="BE5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BF5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BG5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BH5" s="3">
+        <v>1</v>
+      </c>
+      <c r="BI5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="BJ5" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16345872-6E50-0349-9B7A-39BC15B333D4}">
+  <dimension ref="A1:BL6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BJ13" sqref="BJ13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.83203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:64" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" t="s">
+        <v>69</v>
+      </c>
+      <c r="U1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V1" t="s">
+        <v>71</v>
+      </c>
+      <c r="W1" t="s">
+        <v>72</v>
+      </c>
+      <c r="X1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>123</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>125</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>127</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>128</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>129</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>130</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>131</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>132</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>133</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>134</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:64" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AQ3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:64" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>5</v>
+      </c>
+      <c r="AE4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AQ4" s="3">
+        <v>1</v>
+      </c>
+      <c r="BA4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="BB4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="BG4" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:64" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="4">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5">
+        <v>5</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="W5" s="2">
+        <v>3</v>
+      </c>
+      <c r="X5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="4">
+        <v>5</v>
+      </c>
+      <c r="AB5" s="4">
+        <v>5</v>
+      </c>
+      <c r="AD5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AO5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AQ5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AU5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AX5" s="4">
+        <v>5</v>
+      </c>
+      <c r="AY5" s="5">
+        <v>5</v>
+      </c>
+      <c r="BA5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="BD5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="BE5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="BG5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH5" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="BK5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="BL5" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1</v>
+      </c>
+      <c r="M6" s="3">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3">
+        <v>1</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="T6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="U6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB6" s="4">
+        <v>5</v>
+      </c>
+      <c r="AE6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN6" s="2">
+        <v>3</v>
+      </c>
+      <c r="AQ6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AS6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AT6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AU6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AW6" s="4">
+        <v>5</v>
+      </c>
+      <c r="AX6" s="4">
+        <v>5</v>
+      </c>
+      <c r="BA6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="BD6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="BE6" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="BF6" s="21"/>
+      <c r="BG6" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH6" s="21"/>
+      <c r="BI6" s="21"/>
+      <c r="BJ6" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>